<commit_message>
Fix labels in Litneg
</commit_message>
<xml_diff>
--- a/Datasets/negation sentences.xlsx
+++ b/Datasets/negation sentences.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280F63BC-F683-4945-87AE-EAB6500E99D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2AEF78-836A-4EA6-BB87-5691EF94AFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D39CA54-FEC6-4B78-9142-3D58F3F66373}"/>
   </bookViews>
@@ -4149,10 +4149,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4454,7 +4450,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB58ACA-7E64-41D8-B1E3-B036A5C715B9}">
   <dimension ref="A1:K257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4528,7 +4526,7 @@
         <v>1191</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(G2=0,E2,IF(G2=1,F2,""))</f>
+        <f t="shared" ref="J2:J65" si="0">IF(G2=0,E2,IF(G2=1,F2,""))</f>
         <v>She can be trusted</v>
       </c>
       <c r="K2" t="str">
@@ -4565,11 +4563,11 @@
         <v>1192</v>
       </c>
       <c r="J3" t="str">
-        <f>IF(G3=0,E3,IF(G3=1,F3,""))</f>
+        <f t="shared" si="0"/>
         <v>She can not be trusted</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K66" si="0">IF(OR(ISNUMBER(SEARCH("not ",J3)),ISNUMBER(SEARCH("n't ",J3))),"neg","intens")</f>
+        <f t="shared" ref="K3:K66" si="1">IF(OR(ISNUMBER(SEARCH("not ",J3)),ISNUMBER(SEARCH("n't ",J3))),"neg","intens")</f>
         <v>neg</v>
       </c>
     </row>
@@ -4602,11 +4600,11 @@
         <v>1193</v>
       </c>
       <c r="J4" t="str">
-        <f>IF(G4=0,E4,IF(G4=1,F4,""))</f>
+        <f t="shared" si="0"/>
         <v>He was helpful</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(ISNUMBER(SEARCH("not ",J4)),ISNUMBER(SEARCH("n't ",J4))),"neg","intens")</f>
         <v>intens</v>
       </c>
     </row>
@@ -4639,11 +4637,11 @@
         <v>1194</v>
       </c>
       <c r="J5" t="str">
-        <f>IF(G5=0,E5,IF(G5=1,F5,""))</f>
+        <f t="shared" si="0"/>
         <v>he was not helpful</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -4676,11 +4674,11 @@
         <v>1195</v>
       </c>
       <c r="J6" t="str">
-        <f>IF(G6=0,E6,IF(G6=1,F6,""))</f>
+        <f t="shared" si="0"/>
         <v>The man was cool</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -4713,11 +4711,11 @@
         <v>1196</v>
       </c>
       <c r="J7" t="str">
-        <f>IF(G7=0,E7,IF(G7=1,F7,""))</f>
+        <f t="shared" si="0"/>
         <v>The man was not cool</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -4750,11 +4748,11 @@
         <v>1197</v>
       </c>
       <c r="J8" t="str">
-        <f>IF(G8=0,E8,IF(G8=1,F8,""))</f>
+        <f t="shared" si="0"/>
         <v>The child was religious</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -4787,11 +4785,11 @@
         <v>1198</v>
       </c>
       <c r="J9" t="str">
-        <f>IF(G9=0,E9,IF(G9=1,F9,""))</f>
+        <f t="shared" si="0"/>
         <v>The child was not religious</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -4824,11 +4822,11 @@
         <v>1199</v>
       </c>
       <c r="J10" t="str">
-        <f>IF(G10=0,E10,IF(G10=1,F10,""))</f>
+        <f t="shared" si="0"/>
         <v>She felt bad</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -4861,11 +4859,11 @@
         <v>1200</v>
       </c>
       <c r="J11" t="str">
-        <f>IF(G11=0,E11,IF(G11=1,F11,""))</f>
+        <f t="shared" si="0"/>
         <v>She did not feel bad</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -4898,11 +4896,11 @@
         <v>1201</v>
       </c>
       <c r="J12" t="str">
-        <f>IF(G12=0,E12,IF(G12=1,F12,""))</f>
+        <f t="shared" si="0"/>
         <v>The room was open</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -4935,11 +4933,11 @@
         <v>1202</v>
       </c>
       <c r="J13" t="str">
-        <f>IF(G13=0,E13,IF(G13=1,F13,""))</f>
+        <f t="shared" si="0"/>
         <v>The room was not open</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -4972,11 +4970,11 @@
         <v>1203</v>
       </c>
       <c r="J14" t="str">
-        <f>IF(G14=0,E14,IF(G14=1,F14,""))</f>
+        <f t="shared" si="0"/>
         <v>His joints snap</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5009,11 +5007,11 @@
         <v>1204</v>
       </c>
       <c r="J15" t="str">
-        <f>IF(G15=0,E15,IF(G15=1,F15,""))</f>
+        <f t="shared" si="0"/>
         <v>His joints do not snap</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5046,11 +5044,11 @@
         <v>1205</v>
       </c>
       <c r="J16" t="str">
-        <f>IF(G16=0,E16,IF(G16=1,F16,""))</f>
+        <f t="shared" si="0"/>
         <v>The toy was cared for</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5083,11 +5081,11 @@
         <v>1206</v>
       </c>
       <c r="J17" t="str">
-        <f>IF(G17=0,E17,IF(G17=1,F17,""))</f>
+        <f t="shared" si="0"/>
         <v>The toy was not cared for</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5120,11 +5118,11 @@
         <v>1207</v>
       </c>
       <c r="J18" t="str">
-        <f>IF(G18=0,E18,IF(G18=1,F18,""))</f>
+        <f t="shared" si="0"/>
         <v>The movie is funny</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5157,11 +5155,11 @@
         <v>1208</v>
       </c>
       <c r="J19" t="str">
-        <f>IF(G19=0,E19,IF(G19=1,F19,""))</f>
+        <f t="shared" si="0"/>
         <v>The movie is not funny</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5194,11 +5192,11 @@
         <v>1209</v>
       </c>
       <c r="J20" t="str">
-        <f>IF(G20=0,E20,IF(G20=1,F20,""))</f>
+        <f t="shared" si="0"/>
         <v>The couch was comfortable</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5231,11 +5229,11 @@
         <v>1210</v>
       </c>
       <c r="J21" t="str">
-        <f>IF(G21=0,E21,IF(G21=1,F21,""))</f>
+        <f t="shared" si="0"/>
         <v>The couch was not comfortable</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5268,11 +5266,11 @@
         <v>1211</v>
       </c>
       <c r="J22" t="str">
-        <f>IF(G22=0,E22,IF(G22=1,F22,""))</f>
+        <f t="shared" si="0"/>
         <v>The incense smells good</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5305,11 +5303,11 @@
         <v>1212</v>
       </c>
       <c r="J23" t="str">
-        <f>IF(G23=0,E23,IF(G23=1,F23,""))</f>
+        <f t="shared" si="0"/>
         <v>The incense does not smell good</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5342,11 +5340,11 @@
         <v>1213</v>
       </c>
       <c r="J24" t="str">
-        <f>IF(G24=0,E24,IF(G24=1,F24,""))</f>
+        <f t="shared" si="0"/>
         <v>The girl needed water</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5379,11 +5377,11 @@
         <v>1214</v>
       </c>
       <c r="J25" t="str">
-        <f>IF(G25=0,E25,IF(G25=1,F25,""))</f>
+        <f t="shared" si="0"/>
         <v>The girl did not need water</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5416,11 +5414,11 @@
         <v>1215</v>
       </c>
       <c r="J26" t="str">
-        <f>IF(G26=0,E26,IF(G26=1,F26,""))</f>
+        <f t="shared" si="0"/>
         <v>The room was well lit</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5453,11 +5451,11 @@
         <v>1216</v>
       </c>
       <c r="J27" t="str">
-        <f>IF(G27=0,E27,IF(G27=1,F27,""))</f>
+        <f t="shared" si="0"/>
         <v>The room was not well lit</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5490,11 +5488,11 @@
         <v>1217</v>
       </c>
       <c r="J28" t="str">
-        <f>IF(G28=0,E28,IF(G28=1,F28,""))</f>
+        <f t="shared" si="0"/>
         <v>The sun was very bright</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5527,11 +5525,11 @@
         <v>1218</v>
       </c>
       <c r="J29" t="str">
-        <f>IF(G29=0,E29,IF(G29=1,F29,""))</f>
+        <f t="shared" si="0"/>
         <v>The sun was not very bright</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5555,7 +5553,7 @@
         <v>53</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" t="s">
         <v>1241</v>
@@ -5564,12 +5562,12 @@
         <v>1219</v>
       </c>
       <c r="J30" t="str">
-        <f>IF(G30=0,E30,IF(G30=1,F30,""))</f>
-        <v>it's coarse</v>
+        <f t="shared" si="0"/>
+        <v>it's not coarse</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="0"/>
-        <v>intens</v>
+        <f t="shared" si="1"/>
+        <v>neg</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -5592,7 +5590,7 @@
         <v>53</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="s">
         <v>1241</v>
@@ -5601,12 +5599,12 @@
         <v>1220</v>
       </c>
       <c r="J31" t="str">
-        <f>IF(G31=0,E31,IF(G31=1,F31,""))</f>
-        <v>it's not coarse</v>
+        <f t="shared" si="0"/>
+        <v>it's coarse</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="0"/>
-        <v>neg</v>
+        <f t="shared" si="1"/>
+        <v>intens</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -5638,11 +5636,11 @@
         <v>1221</v>
       </c>
       <c r="J32" t="str">
-        <f>IF(G32=0,E32,IF(G32=1,F32,""))</f>
+        <f t="shared" si="0"/>
         <v>She was skillful</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5675,11 +5673,11 @@
         <v>1222</v>
       </c>
       <c r="J33" t="str">
-        <f>IF(G33=0,E33,IF(G33=1,F33,""))</f>
+        <f t="shared" si="0"/>
         <v>She was not skillful</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5712,11 +5710,11 @@
         <v>1223</v>
       </c>
       <c r="J34" t="str">
-        <f>IF(G34=0,E34,IF(G34=1,F34,""))</f>
+        <f t="shared" si="0"/>
         <v>The movie ending made sense</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5749,11 +5747,11 @@
         <v>1224</v>
       </c>
       <c r="J35" t="str">
-        <f>IF(G35=0,E35,IF(G35=1,F35,""))</f>
+        <f t="shared" si="0"/>
         <v>The movie ending did not make sense</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5786,11 +5784,11 @@
         <v>146</v>
       </c>
       <c r="J36" t="str">
-        <f>IF(G36=0,E36,IF(G36=1,F36,""))</f>
+        <f t="shared" si="0"/>
         <v>She wasn't entertaining.</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5823,11 +5821,11 @@
         <v>147</v>
       </c>
       <c r="J37" t="str">
-        <f>IF(G37=0,E37,IF(G37=1,F37,""))</f>
+        <f t="shared" si="0"/>
         <v>She was very entertaining.</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5860,11 +5858,11 @@
         <v>154</v>
       </c>
       <c r="J38" t="str">
-        <f>IF(G38=0,E38,IF(G38=1,F38,""))</f>
+        <f t="shared" si="0"/>
         <v>The cat was furry</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5897,11 +5895,11 @@
         <v>155</v>
       </c>
       <c r="J39" t="str">
-        <f>IF(G39=0,E39,IF(G39=1,F39,""))</f>
+        <f t="shared" si="0"/>
         <v>The cat was not furry</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5934,11 +5932,11 @@
         <v>162</v>
       </c>
       <c r="J40" t="str">
-        <f>IF(G40=0,E40,IF(G40=1,F40,""))</f>
+        <f t="shared" si="0"/>
         <v>The disease was very serious</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -5971,11 +5969,11 @@
         <v>163</v>
       </c>
       <c r="J41" t="str">
-        <f>IF(G41=0,E41,IF(G41=1,F41,""))</f>
+        <f t="shared" si="0"/>
         <v>The disease was not serious</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -5999,7 +5997,7 @@
         <v>181</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="s">
         <v>1247</v>
@@ -6008,12 +6006,12 @@
         <v>169</v>
       </c>
       <c r="J42" t="str">
-        <f>IF(G42=0,E42,IF(G42=1,F42,""))</f>
-        <v>The floor is not slippery</v>
+        <f t="shared" si="0"/>
+        <v>The floor is slippery</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="0"/>
-        <v>neg</v>
+        <f t="shared" si="1"/>
+        <v>intens</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
@@ -6036,7 +6034,7 @@
         <v>181</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="s">
         <v>1247</v>
@@ -6045,12 +6043,12 @@
         <v>170</v>
       </c>
       <c r="J43" t="str">
-        <f>IF(G43=0,E43,IF(G43=1,F43,""))</f>
-        <v>The floor is slippery</v>
+        <f t="shared" si="0"/>
+        <v>The floor is not slippery</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="0"/>
-        <v>intens</v>
+        <f t="shared" si="1"/>
+        <v>neg</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
@@ -6082,11 +6080,11 @@
         <v>179</v>
       </c>
       <c r="J44" t="str">
-        <f>IF(G44=0,E44,IF(G44=1,F44,""))</f>
+        <f t="shared" si="0"/>
         <v>He's busy</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6119,11 +6117,11 @@
         <v>180</v>
       </c>
       <c r="J45" t="str">
-        <f>IF(G45=0,E45,IF(G45=1,F45,""))</f>
+        <f t="shared" si="0"/>
         <v>He's not busy</v>
       </c>
       <c r="K45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6156,11 +6154,11 @@
         <v>190</v>
       </c>
       <c r="J46" t="str">
-        <f>IF(G46=0,E46,IF(G46=1,F46,""))</f>
+        <f t="shared" si="0"/>
         <v>The book is thick</v>
       </c>
       <c r="K46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6193,11 +6191,11 @@
         <v>191</v>
       </c>
       <c r="J47" t="str">
-        <f>IF(G47=0,E47,IF(G47=1,F47,""))</f>
+        <f t="shared" si="0"/>
         <v>The book is not thick</v>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6230,11 +6228,11 @@
         <v>200</v>
       </c>
       <c r="J48" t="str">
-        <f>IF(G48=0,E48,IF(G48=1,F48,""))</f>
+        <f t="shared" si="0"/>
         <v>The man is muscular</v>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6267,11 +6265,11 @@
         <v>201</v>
       </c>
       <c r="J49" t="str">
-        <f>IF(G49=0,E49,IF(G49=1,F49,""))</f>
+        <f t="shared" si="0"/>
         <v>The man is not muscular</v>
       </c>
       <c r="K49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6304,11 +6302,11 @@
         <v>210</v>
       </c>
       <c r="J50" t="str">
-        <f>IF(G50=0,E50,IF(G50=1,F50,""))</f>
+        <f t="shared" si="0"/>
         <v>The computer is fast</v>
       </c>
       <c r="K50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6341,11 +6339,11 @@
         <v>211</v>
       </c>
       <c r="J51" t="str">
-        <f>IF(G51=0,E51,IF(G51=1,F51,""))</f>
+        <f t="shared" si="0"/>
         <v>The computer is not fast</v>
       </c>
       <c r="K51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6378,11 +6376,11 @@
         <v>220</v>
       </c>
       <c r="J52" t="str">
-        <f>IF(G52=0,E52,IF(G52=1,F52,""))</f>
+        <f t="shared" si="0"/>
         <v>He is not brave</v>
       </c>
       <c r="K52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6415,11 +6413,11 @@
         <v>221</v>
       </c>
       <c r="J53" t="str">
-        <f>IF(G53=0,E53,IF(G53=1,F53,""))</f>
+        <f t="shared" si="0"/>
         <v>He is brave</v>
       </c>
       <c r="K53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6452,11 +6450,11 @@
         <v>224</v>
       </c>
       <c r="J54" t="str">
-        <f>IF(G54=0,E54,IF(G54=1,F54,""))</f>
+        <f t="shared" si="0"/>
         <v>The vase is fragile</v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6489,11 +6487,11 @@
         <v>225</v>
       </c>
       <c r="J55" t="str">
-        <f>IF(G55=0,E55,IF(G55=1,F55,""))</f>
+        <f t="shared" si="0"/>
         <v>The vase is not fragile</v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6526,11 +6524,11 @@
         <v>237</v>
       </c>
       <c r="J56" t="str">
-        <f>IF(G56=0,E56,IF(G56=1,F56,""))</f>
+        <f t="shared" si="0"/>
         <v>He knew her well</v>
       </c>
       <c r="K56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6563,11 +6561,11 @@
         <v>238</v>
       </c>
       <c r="J57" t="str">
-        <f>IF(G57=0,E57,IF(G57=1,F57,""))</f>
+        <f t="shared" si="0"/>
         <v>He didn't know her well</v>
       </c>
       <c r="K57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6600,11 +6598,11 @@
         <v>247</v>
       </c>
       <c r="J58" t="str">
-        <f>IF(G58=0,E58,IF(G58=1,F58,""))</f>
+        <f t="shared" si="0"/>
         <v>It wasn't hot</v>
       </c>
       <c r="K58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6637,11 +6635,11 @@
         <v>248</v>
       </c>
       <c r="J59" t="str">
-        <f>IF(G59=0,E59,IF(G59=1,F59,""))</f>
+        <f t="shared" si="0"/>
         <v>It was hot</v>
       </c>
       <c r="K59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6674,11 +6672,11 @@
         <v>257</v>
       </c>
       <c r="J60" t="str">
-        <f>IF(G60=0,E60,IF(G60=1,F60,""))</f>
+        <f t="shared" si="0"/>
         <v>The cat is not hyperactive</v>
       </c>
       <c r="K60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6711,11 +6709,11 @@
         <v>258</v>
       </c>
       <c r="J61" t="str">
-        <f>IF(G61=0,E61,IF(G61=1,F61,""))</f>
+        <f t="shared" si="0"/>
         <v>The cat is hyperactive</v>
       </c>
       <c r="K61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6739,7 +6737,7 @@
         <v>270</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" t="s">
         <v>1257</v>
@@ -6748,12 +6746,12 @@
         <v>266</v>
       </c>
       <c r="J62" t="str">
-        <f>IF(G62=0,E62,IF(G62=1,F62,""))</f>
-        <v>the work was amazing</v>
+        <f t="shared" si="0"/>
+        <v>the work was not amazing</v>
       </c>
       <c r="K62" t="str">
-        <f t="shared" si="0"/>
-        <v>intens</v>
+        <f t="shared" si="1"/>
+        <v>neg</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
@@ -6776,7 +6774,7 @@
         <v>270</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" t="s">
         <v>1257</v>
@@ -6785,12 +6783,12 @@
         <v>267</v>
       </c>
       <c r="J63" t="str">
-        <f>IF(G63=0,E63,IF(G63=1,F63,""))</f>
-        <v>the work was not amazing</v>
+        <f t="shared" si="0"/>
+        <v>the work was amazing</v>
       </c>
       <c r="K63" t="str">
-        <f t="shared" si="0"/>
-        <v>neg</v>
+        <f t="shared" si="1"/>
+        <v>intens</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
@@ -6822,11 +6820,11 @@
         <v>275</v>
       </c>
       <c r="J64" t="str">
-        <f>IF(G64=0,E64,IF(G64=1,F64,""))</f>
+        <f t="shared" si="0"/>
         <v>The child was smart</v>
       </c>
       <c r="K64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6859,11 +6857,11 @@
         <v>276</v>
       </c>
       <c r="J65" t="str">
-        <f>IF(G65=0,E65,IF(G65=1,F65,""))</f>
+        <f t="shared" si="0"/>
         <v>The child was not smart</v>
       </c>
       <c r="K65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>neg</v>
       </c>
     </row>
@@ -6896,11 +6894,11 @@
         <v>284</v>
       </c>
       <c r="J66" t="str">
-        <f>IF(G66=0,E66,IF(G66=1,F66,""))</f>
+        <f t="shared" ref="J66:J129" si="2">IF(G66=0,E66,IF(G66=1,F66,""))</f>
         <v>The government was efficient</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>intens</v>
       </c>
     </row>
@@ -6933,11 +6931,11 @@
         <v>285</v>
       </c>
       <c r="J67" t="str">
-        <f>IF(G67=0,E67,IF(G67=1,F67,""))</f>
+        <f t="shared" si="2"/>
         <v>The government was not efficient</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" ref="K67:K130" si="1">IF(OR(ISNUMBER(SEARCH("not ",J67)),ISNUMBER(SEARCH("n't ",J67))),"neg","intens")</f>
+        <f t="shared" ref="K67:K130" si="3">IF(OR(ISNUMBER(SEARCH("not ",J67)),ISNUMBER(SEARCH("n't ",J67))),"neg","intens")</f>
         <v>neg</v>
       </c>
     </row>
@@ -6970,11 +6968,11 @@
         <v>294</v>
       </c>
       <c r="J68" t="str">
-        <f>IF(G68=0,E68,IF(G68=1,F68,""))</f>
+        <f t="shared" si="2"/>
         <v>She's sweet</v>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7007,11 +7005,11 @@
         <v>295</v>
       </c>
       <c r="J69" t="str">
-        <f>IF(G69=0,E69,IF(G69=1,F69,""))</f>
+        <f t="shared" si="2"/>
         <v>She's not sweet</v>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7044,11 +7042,11 @@
         <v>304</v>
       </c>
       <c r="J70" t="str">
-        <f>IF(G70=0,E70,IF(G70=1,F70,""))</f>
+        <f t="shared" si="2"/>
         <v>The letter was heartwarming.</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7081,11 +7079,11 @@
         <v>305</v>
       </c>
       <c r="J71" t="str">
-        <f>IF(G71=0,E71,IF(G71=1,F71,""))</f>
+        <f t="shared" si="2"/>
         <v>The letter wasn't heartwarming</v>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7118,11 +7116,11 @@
         <v>314</v>
       </c>
       <c r="J72" t="str">
-        <f>IF(G72=0,E72,IF(G72=1,F72,""))</f>
+        <f t="shared" si="2"/>
         <v>The tree canopy does not provide shade</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7155,11 +7153,11 @@
         <v>315</v>
       </c>
       <c r="J73" t="str">
-        <f>IF(G73=0,E73,IF(G73=1,F73,""))</f>
+        <f t="shared" si="2"/>
         <v>The tree canopy provides shade</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7192,11 +7190,11 @@
         <v>322</v>
       </c>
       <c r="J74" t="str">
-        <f>IF(G74=0,E74,IF(G74=1,F74,""))</f>
+        <f t="shared" si="2"/>
         <v>The You Tube tutorial wasn't informative</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7229,11 +7227,11 @@
         <v>323</v>
       </c>
       <c r="J75" t="str">
-        <f>IF(G75=0,E75,IF(G75=1,F75,""))</f>
+        <f t="shared" si="2"/>
         <v>The You Tube tutorial was informative</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7266,11 +7264,11 @@
         <v>332</v>
       </c>
       <c r="J76" t="str">
-        <f>IF(G76=0,E76,IF(G76=1,F76,""))</f>
+        <f t="shared" si="2"/>
         <v>he was scared</v>
       </c>
       <c r="K76" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7303,11 +7301,11 @@
         <v>333</v>
       </c>
       <c r="J77" t="str">
-        <f>IF(G77=0,E77,IF(G77=1,F77,""))</f>
+        <f t="shared" si="2"/>
         <v>he wasn't scared</v>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7340,11 +7338,11 @@
         <v>340</v>
       </c>
       <c r="J78" t="str">
-        <f>IF(G78=0,E78,IF(G78=1,F78,""))</f>
+        <f t="shared" si="2"/>
         <v>It was easy</v>
       </c>
       <c r="K78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7377,11 +7375,11 @@
         <v>341</v>
       </c>
       <c r="J79" t="str">
-        <f>IF(G79=0,E79,IF(G79=1,F79,""))</f>
+        <f t="shared" si="2"/>
         <v>It was not easy</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7414,11 +7412,11 @@
         <v>349</v>
       </c>
       <c r="J80" t="str">
-        <f>IF(G80=0,E80,IF(G80=1,F80,""))</f>
+        <f t="shared" si="2"/>
         <v>The clone is identical</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7451,11 +7449,11 @@
         <v>350</v>
       </c>
       <c r="J81" t="str">
-        <f>IF(G81=0,E81,IF(G81=1,F81,""))</f>
+        <f t="shared" si="2"/>
         <v>The clone isn't identical</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7488,11 +7486,11 @@
         <v>357</v>
       </c>
       <c r="J82" t="str">
-        <f>IF(G82=0,E82,IF(G82=1,F82,""))</f>
+        <f t="shared" si="2"/>
         <v>The weren't close</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7525,11 +7523,11 @@
         <v>358</v>
       </c>
       <c r="J83" t="str">
-        <f>IF(G83=0,E83,IF(G83=1,F83,""))</f>
+        <f t="shared" si="2"/>
         <v>They were close</v>
       </c>
       <c r="K83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7562,11 +7560,11 @@
         <v>367</v>
       </c>
       <c r="J84" t="str">
-        <f>IF(G84=0,E84,IF(G84=1,F84,""))</f>
+        <f t="shared" si="2"/>
         <v>It lives for a long time</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7599,11 +7597,11 @@
         <v>368</v>
       </c>
       <c r="J85" t="str">
-        <f>IF(G85=0,E85,IF(G85=1,F85,""))</f>
+        <f t="shared" si="2"/>
         <v>It doesn't live for a long time</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7636,11 +7634,11 @@
         <v>376</v>
       </c>
       <c r="J86" t="str">
-        <f>IF(G86=0,E86,IF(G86=1,F86,""))</f>
+        <f t="shared" si="2"/>
         <v>It moisturizes well</v>
       </c>
       <c r="K86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7673,11 +7671,11 @@
         <v>377</v>
       </c>
       <c r="J87" t="str">
-        <f>IF(G87=0,E87,IF(G87=1,F87,""))</f>
+        <f t="shared" si="2"/>
         <v>It doesn't moisturize well</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7710,11 +7708,11 @@
         <v>385</v>
       </c>
       <c r="J88" t="str">
-        <f>IF(G88=0,E88,IF(G88=1,F88,""))</f>
+        <f t="shared" si="2"/>
         <v>The movie could be predicted</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7747,11 +7745,11 @@
         <v>386</v>
       </c>
       <c r="J89" t="str">
-        <f>IF(G89=0,E89,IF(G89=1,F89,""))</f>
+        <f t="shared" si="2"/>
         <v>The movie couldn't be predicted</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7784,11 +7782,11 @@
         <v>395</v>
       </c>
       <c r="J90" t="str">
-        <f>IF(G90=0,E90,IF(G90=1,F90,""))</f>
+        <f t="shared" si="2"/>
         <v>The girl gets attention.</v>
       </c>
       <c r="K90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7821,11 +7819,11 @@
         <v>396</v>
       </c>
       <c r="J91" t="str">
-        <f>IF(G91=0,E91,IF(G91=1,F91,""))</f>
+        <f t="shared" si="2"/>
         <v>The girl doesn't get attention</v>
       </c>
       <c r="K91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7858,11 +7856,11 @@
         <v>405</v>
       </c>
       <c r="J92" t="str">
-        <f>IF(G92=0,E92,IF(G92=1,F92,""))</f>
+        <f t="shared" si="2"/>
         <v>Their marriage is very passionate</v>
       </c>
       <c r="K92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -7895,11 +7893,11 @@
         <v>406</v>
       </c>
       <c r="J93" t="str">
-        <f>IF(G93=0,E93,IF(G93=1,F93,""))</f>
+        <f t="shared" si="2"/>
         <v>Their marriage is not very passionate</v>
       </c>
       <c r="K93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7932,11 +7930,11 @@
         <v>415</v>
       </c>
       <c r="J94" t="str">
-        <f>IF(G94=0,E94,IF(G94=1,F94,""))</f>
+        <f t="shared" si="2"/>
         <v>The house was not silent</v>
       </c>
       <c r="K94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -7969,11 +7967,11 @@
         <v>416</v>
       </c>
       <c r="J95" t="str">
-        <f>IF(G95=0,E95,IF(G95=1,F95,""))</f>
+        <f t="shared" si="2"/>
         <v>The house was silent</v>
       </c>
       <c r="K95" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8006,11 +8004,11 @@
         <v>423</v>
       </c>
       <c r="J96" t="str">
-        <f>IF(G96=0,E96,IF(G96=1,F96,""))</f>
+        <f t="shared" si="2"/>
         <v>The pillow is soft</v>
       </c>
       <c r="K96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8043,11 +8041,11 @@
         <v>424</v>
       </c>
       <c r="J97" t="str">
-        <f>IF(G97=0,E97,IF(G97=1,F97,""))</f>
+        <f t="shared" si="2"/>
         <v>The pillow is not soft</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8080,11 +8078,11 @@
         <v>431</v>
       </c>
       <c r="J98" t="str">
-        <f>IF(G98=0,E98,IF(G98=1,F98,""))</f>
+        <f t="shared" si="2"/>
         <v>The book was enjoyable</v>
       </c>
       <c r="K98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8117,11 +8115,11 @@
         <v>432</v>
       </c>
       <c r="J99" t="str">
-        <f>IF(G99=0,E99,IF(G99=1,F99,""))</f>
+        <f t="shared" si="2"/>
         <v>The book was not enjoyable</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8154,11 +8152,11 @@
         <v>439</v>
       </c>
       <c r="J100" t="str">
-        <f>IF(G100=0,E100,IF(G100=1,F100,""))</f>
+        <f t="shared" si="2"/>
         <v>His movements were delicate</v>
       </c>
       <c r="K100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8191,11 +8189,11 @@
         <v>440</v>
       </c>
       <c r="J101" t="str">
-        <f>IF(G101=0,E101,IF(G101=1,F101,""))</f>
+        <f t="shared" si="2"/>
         <v>His movements were not delicate</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8228,11 +8226,11 @@
         <v>447</v>
       </c>
       <c r="J102" t="str">
-        <f>IF(G102=0,E102,IF(G102=1,F102,""))</f>
+        <f t="shared" si="2"/>
         <v>The light was bright</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8265,11 +8263,11 @@
         <v>448</v>
       </c>
       <c r="J103" t="str">
-        <f>IF(G103=0,E103,IF(G103=1,F103,""))</f>
+        <f t="shared" si="2"/>
         <v>The light was not bright</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8302,11 +8300,11 @@
         <v>455</v>
       </c>
       <c r="J104" t="str">
-        <f>IF(G104=0,E104,IF(G104=1,F104,""))</f>
+        <f t="shared" si="2"/>
         <v>The bottle is clear</v>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8339,11 +8337,11 @@
         <v>456</v>
       </c>
       <c r="J105" t="str">
-        <f>IF(G105=0,E105,IF(G105=1,F105,""))</f>
+        <f t="shared" si="2"/>
         <v>The bottle is not clear</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8376,11 +8374,11 @@
         <v>465</v>
       </c>
       <c r="J106" t="str">
-        <f>IF(G106=0,E106,IF(G106=1,F106,""))</f>
+        <f t="shared" si="2"/>
         <v>The cat was deadly</v>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8413,11 +8411,11 @@
         <v>466</v>
       </c>
       <c r="J107" t="str">
-        <f>IF(G107=0,E107,IF(G107=1,F107,""))</f>
+        <f t="shared" si="2"/>
         <v>The cat was not deadly</v>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8450,11 +8448,11 @@
         <v>475</v>
       </c>
       <c r="J108" t="str">
-        <f>IF(G108=0,E108,IF(G108=1,F108,""))</f>
+        <f t="shared" si="2"/>
         <v>The actors are not talented</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8487,11 +8485,11 @@
         <v>476</v>
       </c>
       <c r="J109" t="str">
-        <f>IF(G109=0,E109,IF(G109=1,F109,""))</f>
+        <f t="shared" si="2"/>
         <v>The actors are very talented</v>
       </c>
       <c r="K109" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8524,11 +8522,11 @@
         <v>483</v>
       </c>
       <c r="J110" t="str">
-        <f>IF(G110=0,E110,IF(G110=1,F110,""))</f>
+        <f t="shared" si="2"/>
         <v>The tofu is spicy</v>
       </c>
       <c r="K110" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8561,11 +8559,11 @@
         <v>484</v>
       </c>
       <c r="J111" t="str">
-        <f>IF(G111=0,E111,IF(G111=1,F111,""))</f>
+        <f t="shared" si="2"/>
         <v>The tofu is not spicy</v>
       </c>
       <c r="K111" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8598,11 +8596,11 @@
         <v>493</v>
       </c>
       <c r="J112" t="str">
-        <f>IF(G112=0,E112,IF(G112=1,F112,""))</f>
+        <f t="shared" si="2"/>
         <v>The car works well</v>
       </c>
       <c r="K112" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8635,11 +8633,11 @@
         <v>494</v>
       </c>
       <c r="J113" t="str">
-        <f>IF(G113=0,E113,IF(G113=1,F113,""))</f>
+        <f t="shared" si="2"/>
         <v>The car does not work well</v>
       </c>
       <c r="K113" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8672,11 +8670,11 @@
         <v>501</v>
       </c>
       <c r="J114" t="str">
-        <f>IF(G114=0,E114,IF(G114=1,F114,""))</f>
+        <f t="shared" si="2"/>
         <v>The woman is good looking</v>
       </c>
       <c r="K114" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8709,11 +8707,11 @@
         <v>502</v>
       </c>
       <c r="J115" t="str">
-        <f>IF(G115=0,E115,IF(G115=1,F115,""))</f>
+        <f t="shared" si="2"/>
         <v>The woman is not good looking</v>
       </c>
       <c r="K115" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8746,11 +8744,11 @@
         <v>511</v>
       </c>
       <c r="J116" t="str">
-        <f>IF(G116=0,E116,IF(G116=1,F116,""))</f>
+        <f t="shared" si="2"/>
         <v>The drawing was round</v>
       </c>
       <c r="K116" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8783,11 +8781,11 @@
         <v>512</v>
       </c>
       <c r="J117" t="str">
-        <f>IF(G117=0,E117,IF(G117=1,F117,""))</f>
+        <f t="shared" si="2"/>
         <v>The drawing was not round</v>
       </c>
       <c r="K117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8820,11 +8818,11 @@
         <v>521</v>
       </c>
       <c r="J118" t="str">
-        <f>IF(G118=0,E118,IF(G118=1,F118,""))</f>
+        <f t="shared" si="2"/>
         <v>I am very hungry</v>
       </c>
       <c r="K118" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8857,11 +8855,11 @@
         <v>522</v>
       </c>
       <c r="J119" t="str">
-        <f>IF(G119=0,E119,IF(G119=1,F119,""))</f>
+        <f t="shared" si="2"/>
         <v>I am not very hungry</v>
       </c>
       <c r="K119" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8894,11 +8892,11 @@
         <v>531</v>
       </c>
       <c r="J120" t="str">
-        <f>IF(G120=0,E120,IF(G120=1,F120,""))</f>
+        <f t="shared" si="2"/>
         <v>He is not sociable</v>
       </c>
       <c r="K120" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -8931,11 +8929,11 @@
         <v>532</v>
       </c>
       <c r="J121" t="str">
-        <f>IF(G121=0,E121,IF(G121=1,F121,""))</f>
+        <f t="shared" si="2"/>
         <v>He is sociable</v>
       </c>
       <c r="K121" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -8968,11 +8966,11 @@
         <v>541</v>
       </c>
       <c r="J122" t="str">
-        <f>IF(G122=0,E122,IF(G122=1,F122,""))</f>
+        <f t="shared" si="2"/>
         <v>The juice box is sticky</v>
       </c>
       <c r="K122" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -9005,11 +9003,11 @@
         <v>542</v>
       </c>
       <c r="J123" t="str">
-        <f>IF(G123=0,E123,IF(G123=1,F123,""))</f>
+        <f t="shared" si="2"/>
         <v>The juice box isn't sticky</v>
       </c>
       <c r="K123" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -9042,11 +9040,11 @@
         <v>550</v>
       </c>
       <c r="J124" t="str">
-        <f>IF(G124=0,E124,IF(G124=1,F124,""))</f>
+        <f t="shared" si="2"/>
         <v>The lightbulb puts out a lot of light</v>
       </c>
       <c r="K124" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -9079,11 +9077,11 @@
         <v>551</v>
       </c>
       <c r="J125" t="str">
-        <f>IF(G125=0,E125,IF(G125=1,F125,""))</f>
+        <f t="shared" si="2"/>
         <v>The lightbulb does not put out a lot of light</v>
       </c>
       <c r="K125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -9116,11 +9114,11 @@
         <v>560</v>
       </c>
       <c r="J126" t="str">
-        <f>IF(G126=0,E126,IF(G126=1,F126,""))</f>
+        <f t="shared" si="2"/>
         <v>The screen play wasn't realistic</v>
       </c>
       <c r="K126" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -9153,11 +9151,11 @@
         <v>561</v>
       </c>
       <c r="J127" t="str">
-        <f>IF(G127=0,E127,IF(G127=1,F127,""))</f>
+        <f t="shared" si="2"/>
         <v>The screen play was very factual</v>
       </c>
       <c r="K127" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -9190,11 +9188,11 @@
         <v>569</v>
       </c>
       <c r="J128" t="str">
-        <f>IF(G128=0,E128,IF(G128=1,F128,""))</f>
+        <f t="shared" si="2"/>
         <v>he book was not fantastic</v>
       </c>
       <c r="K128" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -9227,11 +9225,11 @@
         <v>570</v>
       </c>
       <c r="J129" t="str">
-        <f>IF(G129=0,E129,IF(G129=1,F129,""))</f>
+        <f t="shared" si="2"/>
         <v>The book was fantastic</v>
       </c>
       <c r="K129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>intens</v>
       </c>
     </row>
@@ -9264,11 +9262,11 @@
         <v>579</v>
       </c>
       <c r="J130" t="str">
-        <f>IF(G130=0,E130,IF(G130=1,F130,""))</f>
+        <f t="shared" ref="J130:J193" si="4">IF(G130=0,E130,IF(G130=1,F130,""))</f>
         <v>My puppy doesn't have a lot of energy</v>
       </c>
       <c r="K130" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>neg</v>
       </c>
     </row>
@@ -9301,11 +9299,11 @@
         <v>580</v>
       </c>
       <c r="J131" t="str">
-        <f>IF(G131=0,E131,IF(G131=1,F131,""))</f>
+        <f t="shared" si="4"/>
         <v>My puppy has a lot of energy</v>
       </c>
       <c r="K131" t="str">
-        <f t="shared" ref="K131:K194" si="2">IF(OR(ISNUMBER(SEARCH("not ",J131)),ISNUMBER(SEARCH("n't ",J131))),"neg","intens")</f>
+        <f t="shared" ref="K131:K194" si="5">IF(OR(ISNUMBER(SEARCH("not ",J131)),ISNUMBER(SEARCH("n't ",J131))),"neg","intens")</f>
         <v>intens</v>
       </c>
     </row>
@@ -9338,11 +9336,11 @@
         <v>587</v>
       </c>
       <c r="J132" t="str">
-        <f>IF(G132=0,E132,IF(G132=1,F132,""))</f>
+        <f t="shared" si="4"/>
         <v>She was not interesting</v>
       </c>
       <c r="K132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -9375,11 +9373,11 @@
         <v>588</v>
       </c>
       <c r="J133" t="str">
-        <f>IF(G133=0,E133,IF(G133=1,F133,""))</f>
+        <f t="shared" si="4"/>
         <v>She was interesting</v>
       </c>
       <c r="K133" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9412,11 +9410,11 @@
         <v>596</v>
       </c>
       <c r="J134" t="str">
-        <f>IF(G134=0,E134,IF(G134=1,F134,""))</f>
+        <f t="shared" si="4"/>
         <v>The peppers were hot</v>
       </c>
       <c r="K134" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9449,11 +9447,11 @@
         <v>597</v>
       </c>
       <c r="J135" t="str">
-        <f>IF(G135=0,E135,IF(G135=1,F135,""))</f>
+        <f t="shared" si="4"/>
         <v>The peppers were not hot</v>
       </c>
       <c r="K135" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -9486,11 +9484,11 @@
         <v>606</v>
       </c>
       <c r="J136" t="str">
-        <f>IF(G136=0,E136,IF(G136=1,F136,""))</f>
+        <f t="shared" si="4"/>
         <v>Her fingernails were brittle</v>
       </c>
       <c r="K136" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9523,11 +9521,11 @@
         <v>607</v>
       </c>
       <c r="J137" t="str">
-        <f>IF(G137=0,E137,IF(G137=1,F137,""))</f>
+        <f t="shared" si="4"/>
         <v>Her fingernails were not brittle</v>
       </c>
       <c r="K137" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -9560,11 +9558,11 @@
         <v>614</v>
       </c>
       <c r="J138" t="str">
-        <f>IF(G138=0,E138,IF(G138=1,F138,""))</f>
+        <f t="shared" si="4"/>
         <v>He can run really fast</v>
       </c>
       <c r="K138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9597,11 +9595,11 @@
         <v>615</v>
       </c>
       <c r="J139" t="str">
-        <f>IF(G139=0,E139,IF(G139=1,F139,""))</f>
+        <f t="shared" si="4"/>
         <v>He can not run really fast</v>
       </c>
       <c r="K139" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -9634,11 +9632,11 @@
         <v>625</v>
       </c>
       <c r="J140" t="str">
-        <f>IF(G140=0,E140,IF(G140=1,F140,""))</f>
+        <f t="shared" si="4"/>
         <v>The movie was funny</v>
       </c>
       <c r="K140" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9671,11 +9669,11 @@
         <v>624</v>
       </c>
       <c r="J141" t="str">
-        <f>IF(G141=0,E141,IF(G141=1,F141,""))</f>
+        <f t="shared" si="4"/>
         <v>The movie wasn't funny</v>
       </c>
       <c r="K141" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -9708,11 +9706,11 @@
         <v>634</v>
       </c>
       <c r="J142" t="str">
-        <f>IF(G142=0,E142,IF(G142=1,F142,""))</f>
+        <f t="shared" si="4"/>
         <v>The fence is rusty</v>
       </c>
       <c r="K142" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9745,11 +9743,11 @@
         <v>635</v>
       </c>
       <c r="J143" t="str">
-        <f>IF(G143=0,E143,IF(G143=1,F143,""))</f>
+        <f t="shared" si="4"/>
         <v>The fence is not rusty</v>
       </c>
       <c r="K143" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -9782,11 +9780,11 @@
         <v>643</v>
       </c>
       <c r="J144" t="str">
-        <f>IF(G144=0,E144,IF(G144=1,F144,""))</f>
+        <f t="shared" si="4"/>
         <v>The movie was long</v>
       </c>
       <c r="K144" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9819,11 +9817,11 @@
         <v>644</v>
       </c>
       <c r="J145" t="str">
-        <f>IF(G145=0,E145,IF(G145=1,F145,""))</f>
+        <f t="shared" si="4"/>
         <v>The movie was not long</v>
       </c>
       <c r="K145" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -9856,11 +9854,11 @@
         <v>653</v>
       </c>
       <c r="J146" t="str">
-        <f>IF(G146=0,E146,IF(G146=1,F146,""))</f>
+        <f t="shared" si="4"/>
         <v>She was not emotionally resilient</v>
       </c>
       <c r="K146" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -9893,11 +9891,11 @@
         <v>654</v>
       </c>
       <c r="J147" t="str">
-        <f>IF(G147=0,E147,IF(G147=1,F147,""))</f>
+        <f t="shared" si="4"/>
         <v>She was emotionally resilient</v>
       </c>
       <c r="K147" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9930,11 +9928,11 @@
         <v>663</v>
       </c>
       <c r="J148" t="str">
-        <f>IF(G148=0,E148,IF(G148=1,F148,""))</f>
+        <f t="shared" si="4"/>
         <v>The item is valuable</v>
       </c>
       <c r="K148" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -9967,11 +9965,11 @@
         <v>664</v>
       </c>
       <c r="J149" t="str">
-        <f>IF(G149=0,E149,IF(G149=1,F149,""))</f>
+        <f t="shared" si="4"/>
         <v>The item is not valuable</v>
       </c>
       <c r="K149" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10004,11 +10002,11 @@
         <v>673</v>
       </c>
       <c r="J150" t="str">
-        <f>IF(G150=0,E150,IF(G150=1,F150,""))</f>
+        <f t="shared" si="4"/>
         <v>His position was not stable</v>
       </c>
       <c r="K150" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10041,11 +10039,11 @@
         <v>674</v>
       </c>
       <c r="J151" t="str">
-        <f>IF(G151=0,E151,IF(G151=1,F151,""))</f>
+        <f t="shared" si="4"/>
         <v>His position was stable</v>
       </c>
       <c r="K151" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10078,11 +10076,11 @@
         <v>683</v>
       </c>
       <c r="J152" t="str">
-        <f>IF(G152=0,E152,IF(G152=1,F152,""))</f>
+        <f t="shared" si="4"/>
         <v>His feet were not small</v>
       </c>
       <c r="K152" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10115,11 +10113,11 @@
         <v>684</v>
       </c>
       <c r="J153" t="str">
-        <f>IF(G153=0,E153,IF(G153=1,F153,""))</f>
+        <f t="shared" si="4"/>
         <v>His feet were small</v>
       </c>
       <c r="K153" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10152,11 +10150,11 @@
         <v>693</v>
       </c>
       <c r="J154" t="str">
-        <f>IF(G154=0,E154,IF(G154=1,F154,""))</f>
+        <f t="shared" si="4"/>
         <v>The gift was beneficial</v>
       </c>
       <c r="K154" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10189,11 +10187,11 @@
         <v>694</v>
       </c>
       <c r="J155" t="str">
-        <f>IF(G155=0,E155,IF(G155=1,F155,""))</f>
+        <f t="shared" si="4"/>
         <v>The gift was not beneficial</v>
       </c>
       <c r="K155" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10226,11 +10224,11 @@
         <v>703</v>
       </c>
       <c r="J156" t="str">
-        <f>IF(G156=0,E156,IF(G156=1,F156,""))</f>
+        <f t="shared" si="4"/>
         <v>The man is ambitious</v>
       </c>
       <c r="K156" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10263,11 +10261,11 @@
         <v>704</v>
       </c>
       <c r="J157" t="str">
-        <f>IF(G157=0,E157,IF(G157=1,F157,""))</f>
+        <f t="shared" si="4"/>
         <v>The man is not ambitious</v>
       </c>
       <c r="K157" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10300,11 +10298,11 @@
         <v>713</v>
       </c>
       <c r="J158" t="str">
-        <f>IF(G158=0,E158,IF(G158=1,F158,""))</f>
+        <f t="shared" si="4"/>
         <v>The game is very hard</v>
       </c>
       <c r="K158" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10337,11 +10335,11 @@
         <v>714</v>
       </c>
       <c r="J159" t="str">
-        <f>IF(G159=0,E159,IF(G159=1,F159,""))</f>
+        <f t="shared" si="4"/>
         <v>The game is not very hard</v>
       </c>
       <c r="K159" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10374,11 +10372,11 @@
         <v>722</v>
       </c>
       <c r="J160" t="str">
-        <f>IF(G160=0,E160,IF(G160=1,F160,""))</f>
+        <f t="shared" si="4"/>
         <v>The boy's voice could be heard</v>
       </c>
       <c r="K160" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10411,11 +10409,11 @@
         <v>723</v>
       </c>
       <c r="J161" t="str">
-        <f>IF(G161=0,E161,IF(G161=1,F161,""))</f>
+        <f t="shared" si="4"/>
         <v>The boy's voice couldn't be heard</v>
       </c>
       <c r="K161" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10448,11 +10446,11 @@
         <v>732</v>
       </c>
       <c r="J162" t="str">
-        <f>IF(G162=0,E162,IF(G162=1,F162,""))</f>
+        <f t="shared" si="4"/>
         <v>He sees well</v>
       </c>
       <c r="K162" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10485,11 +10483,11 @@
         <v>733</v>
       </c>
       <c r="J163" t="str">
-        <f>IF(G163=0,E163,IF(G163=1,F163,""))</f>
+        <f t="shared" si="4"/>
         <v>He doesn't see well</v>
       </c>
       <c r="K163" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10522,11 +10520,11 @@
         <v>741</v>
       </c>
       <c r="J164" t="str">
-        <f>IF(G164=0,E164,IF(G164=1,F164,""))</f>
+        <f t="shared" si="4"/>
         <v>He's not lenient</v>
       </c>
       <c r="K164" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10559,11 +10557,11 @@
         <v>742</v>
       </c>
       <c r="J165" t="str">
-        <f>IF(G165=0,E165,IF(G165=1,F165,""))</f>
+        <f t="shared" si="4"/>
         <v>He's lenient</v>
       </c>
       <c r="K165" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10596,11 +10594,11 @@
         <v>751</v>
       </c>
       <c r="J166" t="str">
-        <f>IF(G166=0,E166,IF(G166=1,F166,""))</f>
+        <f t="shared" si="4"/>
         <v>The comedian was funny</v>
       </c>
       <c r="K166" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10633,11 +10631,11 @@
         <v>752</v>
       </c>
       <c r="J167" t="str">
-        <f>IF(G167=0,E167,IF(G167=1,F167,""))</f>
+        <f t="shared" si="4"/>
         <v>The comedian was not funny</v>
       </c>
       <c r="K167" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10670,11 +10668,11 @@
         <v>759</v>
       </c>
       <c r="J168" t="str">
-        <f>IF(G168=0,E168,IF(G168=1,F168,""))</f>
+        <f t="shared" si="4"/>
         <v>The judge is not smart</v>
       </c>
       <c r="K168" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10707,11 +10705,11 @@
         <v>760</v>
       </c>
       <c r="J169" t="str">
-        <f>IF(G169=0,E169,IF(G169=1,F169,""))</f>
+        <f t="shared" si="4"/>
         <v>The judge is smart</v>
       </c>
       <c r="K169" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10744,11 +10742,11 @@
         <v>769</v>
       </c>
       <c r="J170" t="str">
-        <f>IF(G170=0,E170,IF(G170=1,F170,""))</f>
+        <f t="shared" si="4"/>
         <v>The wave was very big</v>
       </c>
       <c r="K170" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10781,11 +10779,11 @@
         <v>770</v>
       </c>
       <c r="J171" t="str">
-        <f>IF(G171=0,E171,IF(G171=1,F171,""))</f>
+        <f t="shared" si="4"/>
         <v>The wave wasn't very big</v>
       </c>
       <c r="K171" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10818,11 +10816,11 @@
         <v>779</v>
       </c>
       <c r="J172" t="str">
-        <f>IF(G172=0,E172,IF(G172=1,F172,""))</f>
+        <f t="shared" si="4"/>
         <v>It's fun</v>
       </c>
       <c r="K172" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10855,11 +10853,11 @@
         <v>780</v>
       </c>
       <c r="J173" t="str">
-        <f>IF(G173=0,E173,IF(G173=1,F173,""))</f>
+        <f t="shared" si="4"/>
         <v>It's not fun</v>
       </c>
       <c r="K173" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10892,11 +10890,11 @@
         <v>789</v>
       </c>
       <c r="J174" t="str">
-        <f>IF(G174=0,E174,IF(G174=1,F174,""))</f>
+        <f t="shared" si="4"/>
         <v>The shopping list was detailed</v>
       </c>
       <c r="K174" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -10929,11 +10927,11 @@
         <v>790</v>
       </c>
       <c r="J175" t="str">
-        <f>IF(G175=0,E175,IF(G175=1,F175,""))</f>
+        <f t="shared" si="4"/>
         <v>The shopping list was not detailed</v>
       </c>
       <c r="K175" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -10966,11 +10964,11 @@
         <v>799</v>
       </c>
       <c r="J176" t="str">
-        <f>IF(G176=0,E176,IF(G176=1,F176,""))</f>
+        <f t="shared" si="4"/>
         <v>The blanket was soft</v>
       </c>
       <c r="K176" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11003,11 +11001,11 @@
         <v>800</v>
       </c>
       <c r="J177" t="str">
-        <f>IF(G177=0,E177,IF(G177=1,F177,""))</f>
+        <f t="shared" si="4"/>
         <v>The blanket was not soft</v>
       </c>
       <c r="K177" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11040,11 +11038,11 @@
         <v>809</v>
       </c>
       <c r="J178" t="str">
-        <f>IF(G178=0,E178,IF(G178=1,F178,""))</f>
+        <f t="shared" si="4"/>
         <v>He was emotional while singing</v>
       </c>
       <c r="K178" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11077,11 +11075,11 @@
         <v>810</v>
       </c>
       <c r="J179" t="str">
-        <f>IF(G179=0,E179,IF(G179=1,F179,""))</f>
+        <f t="shared" si="4"/>
         <v>He was not emotional while singing</v>
       </c>
       <c r="K179" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11114,11 +11112,11 @@
         <v>819</v>
       </c>
       <c r="J180" t="str">
-        <f>IF(G180=0,E180,IF(G180=1,F180,""))</f>
+        <f t="shared" si="4"/>
         <v>The football fans believed that the football season would be successful</v>
       </c>
       <c r="K180" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11151,11 +11149,11 @@
         <v>820</v>
       </c>
       <c r="J181" t="str">
-        <f>IF(G181=0,E181,IF(G181=1,F181,""))</f>
+        <f t="shared" si="4"/>
         <v>The football fans did not believe that the football season would be successful</v>
       </c>
       <c r="K181" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11188,11 +11186,11 @@
         <v>829</v>
       </c>
       <c r="J182" t="str">
-        <f>IF(G182=0,E182,IF(G182=1,F182,""))</f>
+        <f t="shared" si="4"/>
         <v>The girl's smile was exuberant</v>
       </c>
       <c r="K182" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11225,11 +11223,11 @@
         <v>830</v>
       </c>
       <c r="J183" t="str">
-        <f>IF(G183=0,E183,IF(G183=1,F183,""))</f>
+        <f t="shared" si="4"/>
         <v>The girl's smile was not exuberant</v>
       </c>
       <c r="K183" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11262,11 +11260,11 @@
         <v>840</v>
       </c>
       <c r="J184" t="str">
-        <f>IF(G184=0,E184,IF(G184=1,F184,""))</f>
+        <f t="shared" si="4"/>
         <v>He was charming</v>
       </c>
       <c r="K184" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11299,11 +11297,11 @@
         <v>839</v>
       </c>
       <c r="J185" t="str">
-        <f>IF(G185=0,E185,IF(G185=1,F185,""))</f>
+        <f t="shared" si="4"/>
         <v>He was not charming</v>
       </c>
       <c r="K185" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11336,11 +11334,11 @@
         <v>849</v>
       </c>
       <c r="J186" t="str">
-        <f>IF(G186=0,E186,IF(G186=1,F186,""))</f>
+        <f t="shared" si="4"/>
         <v>He doesn't share a lot</v>
       </c>
       <c r="K186" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11373,11 +11371,11 @@
         <v>850</v>
       </c>
       <c r="J187" t="str">
-        <f>IF(G187=0,E187,IF(G187=1,F187,""))</f>
+        <f t="shared" si="4"/>
         <v>He shares a lot</v>
       </c>
       <c r="K187" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11410,11 +11408,11 @@
         <v>857</v>
       </c>
       <c r="J188" t="str">
-        <f>IF(G188=0,E188,IF(G188=1,F188,""))</f>
+        <f t="shared" si="4"/>
         <v>This food is very flavorful</v>
       </c>
       <c r="K188" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11447,11 +11445,11 @@
         <v>858</v>
       </c>
       <c r="J189" t="str">
-        <f>IF(G189=0,E189,IF(G189=1,F189,""))</f>
+        <f t="shared" si="4"/>
         <v>This food is not very flavorful</v>
       </c>
       <c r="K189" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11484,11 +11482,11 @@
         <v>869</v>
       </c>
       <c r="J190" t="str">
-        <f>IF(G190=0,E190,IF(G190=1,F190,""))</f>
+        <f t="shared" si="4"/>
         <v>This hurts</v>
       </c>
       <c r="K190" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11521,11 +11519,11 @@
         <v>870</v>
       </c>
       <c r="J191" t="str">
-        <f>IF(G191=0,E191,IF(G191=1,F191,""))</f>
+        <f t="shared" si="4"/>
         <v>This does not hurt</v>
       </c>
       <c r="K191" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11558,11 +11556,11 @@
         <v>879</v>
       </c>
       <c r="J192" t="str">
-        <f>IF(G192=0,E192,IF(G192=1,F192,""))</f>
+        <f t="shared" si="4"/>
         <v>The knife is shiny</v>
       </c>
       <c r="K192" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11595,11 +11593,11 @@
         <v>880</v>
       </c>
       <c r="J193" t="str">
-        <f>IF(G193=0,E193,IF(G193=1,F193,""))</f>
+        <f t="shared" si="4"/>
         <v>The knife is not shiny</v>
       </c>
       <c r="K193" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>neg</v>
       </c>
     </row>
@@ -11632,11 +11630,11 @@
         <v>888</v>
       </c>
       <c r="J194" t="str">
-        <f>IF(G194=0,E194,IF(G194=1,F194,""))</f>
+        <f t="shared" ref="J194:J257" si="6">IF(G194=0,E194,IF(G194=1,F194,""))</f>
         <v>The bone is white</v>
       </c>
       <c r="K194" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>intens</v>
       </c>
     </row>
@@ -11669,11 +11667,11 @@
         <v>889</v>
       </c>
       <c r="J195" t="str">
-        <f>IF(G195=0,E195,IF(G195=1,F195,""))</f>
+        <f t="shared" si="6"/>
         <v>The bone is not white</v>
       </c>
       <c r="K195" t="str">
-        <f t="shared" ref="K195:K257" si="3">IF(OR(ISNUMBER(SEARCH("not ",J195)),ISNUMBER(SEARCH("n't ",J195))),"neg","intens")</f>
+        <f t="shared" ref="K195:K257" si="7">IF(OR(ISNUMBER(SEARCH("not ",J195)),ISNUMBER(SEARCH("n't ",J195))),"neg","intens")</f>
         <v>neg</v>
       </c>
     </row>
@@ -11706,11 +11704,11 @@
         <v>897</v>
       </c>
       <c r="J196" t="str">
-        <f>IF(G196=0,E196,IF(G196=1,F196,""))</f>
+        <f t="shared" si="6"/>
         <v>The villain is a genius</v>
       </c>
       <c r="K196" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -11743,11 +11741,11 @@
         <v>898</v>
       </c>
       <c r="J197" t="str">
-        <f>IF(G197=0,E197,IF(G197=1,F197,""))</f>
+        <f t="shared" si="6"/>
         <v>The villain is not a genius</v>
       </c>
       <c r="K197" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -11780,11 +11778,11 @@
         <v>906</v>
       </c>
       <c r="J198" t="str">
-        <f>IF(G198=0,E198,IF(G198=1,F198,""))</f>
+        <f t="shared" si="6"/>
         <v>He knows a lot about science</v>
       </c>
       <c r="K198" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -11817,11 +11815,11 @@
         <v>907</v>
       </c>
       <c r="J199" t="str">
-        <f>IF(G199=0,E199,IF(G199=1,F199,""))</f>
+        <f t="shared" si="6"/>
         <v>He doesn't know a lot about science</v>
       </c>
       <c r="K199" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -11854,11 +11852,11 @@
         <v>916</v>
       </c>
       <c r="J200" t="str">
-        <f>IF(G200=0,E200,IF(G200=1,F200,""))</f>
+        <f t="shared" si="6"/>
         <v>The man is honest</v>
       </c>
       <c r="K200" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -11891,11 +11889,11 @@
         <v>917</v>
       </c>
       <c r="J201" t="str">
-        <f>IF(G201=0,E201,IF(G201=1,F201,""))</f>
+        <f t="shared" si="6"/>
         <v>The man is not honest</v>
       </c>
       <c r="K201" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -11928,11 +11926,11 @@
         <v>926</v>
       </c>
       <c r="J202" t="str">
-        <f>IF(G202=0,E202,IF(G202=1,F202,""))</f>
+        <f t="shared" si="6"/>
         <v>He fought well</v>
       </c>
       <c r="K202" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -11965,11 +11963,11 @@
         <v>927</v>
       </c>
       <c r="J203" t="str">
-        <f>IF(G203=0,E203,IF(G203=1,F203,""))</f>
+        <f t="shared" si="6"/>
         <v>He didn't fight well</v>
       </c>
       <c r="K203" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12002,11 +12000,11 @@
         <v>936</v>
       </c>
       <c r="J204" t="str">
-        <f>IF(G204=0,E204,IF(G204=1,F204,""))</f>
+        <f t="shared" si="6"/>
         <v>The house was inviting</v>
       </c>
       <c r="K204" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12039,11 +12037,11 @@
         <v>937</v>
       </c>
       <c r="J205" t="str">
-        <f>IF(G205=0,E205,IF(G205=1,F205,""))</f>
+        <f t="shared" si="6"/>
         <v>The house was not inviting</v>
       </c>
       <c r="K205" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12076,11 +12074,11 @@
         <v>947</v>
       </c>
       <c r="J206" t="str">
-        <f>IF(G206=0,E206,IF(G206=1,F206,""))</f>
+        <f t="shared" si="6"/>
         <v>The website was useful</v>
       </c>
       <c r="K206" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12113,11 +12111,11 @@
         <v>946</v>
       </c>
       <c r="J207" t="str">
-        <f>IF(G207=0,E207,IF(G207=1,F207,""))</f>
+        <f t="shared" si="6"/>
         <v>The website was not useful</v>
       </c>
       <c r="K207" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12150,11 +12148,11 @@
         <v>956</v>
       </c>
       <c r="J208" t="str">
-        <f>IF(G208=0,E208,IF(G208=1,F208,""))</f>
+        <f t="shared" si="6"/>
         <v>The lamp gave off a lot of light</v>
       </c>
       <c r="K208" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12187,11 +12185,11 @@
         <v>957</v>
       </c>
       <c r="J209" t="str">
-        <f>IF(G209=0,E209,IF(G209=1,F209,""))</f>
+        <f t="shared" si="6"/>
         <v>The lamp did not give off a lot of light</v>
       </c>
       <c r="K209" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12224,11 +12222,11 @@
         <v>965</v>
       </c>
       <c r="J210" t="str">
-        <f>IF(G210=0,E210,IF(G210=1,F210,""))</f>
+        <f t="shared" si="6"/>
         <v>The costume fit well</v>
       </c>
       <c r="K210" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12261,11 +12259,11 @@
         <v>966</v>
       </c>
       <c r="J211" t="str">
-        <f>IF(G211=0,E211,IF(G211=1,F211,""))</f>
+        <f t="shared" si="6"/>
         <v>The costume didn't fit well</v>
       </c>
       <c r="K211" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12298,11 +12296,11 @@
         <v>975</v>
       </c>
       <c r="J212" t="str">
-        <f>IF(G212=0,E212,IF(G212=1,F212,""))</f>
+        <f t="shared" si="6"/>
         <v>There's not many people interested in this</v>
       </c>
       <c r="K212" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12335,11 +12333,11 @@
         <v>976</v>
       </c>
       <c r="J213" t="str">
-        <f>IF(G213=0,E213,IF(G213=1,F213,""))</f>
+        <f t="shared" si="6"/>
         <v>There's many people interested in this</v>
       </c>
       <c r="K213" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12372,11 +12370,11 @@
         <v>985</v>
       </c>
       <c r="J214" t="str">
-        <f>IF(G214=0,E214,IF(G214=1,F214,""))</f>
+        <f t="shared" si="6"/>
         <v>The boy is thin</v>
       </c>
       <c r="K214" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12409,11 +12407,11 @@
         <v>986</v>
       </c>
       <c r="J215" t="str">
-        <f>IF(G215=0,E215,IF(G215=1,F215,""))</f>
+        <f t="shared" si="6"/>
         <v>The boy isn't thin</v>
       </c>
       <c r="K215" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12446,11 +12444,11 @@
         <v>995</v>
       </c>
       <c r="J216" t="str">
-        <f>IF(G216=0,E216,IF(G216=1,F216,""))</f>
+        <f t="shared" si="6"/>
         <v>The artist's work is recognizable</v>
       </c>
       <c r="K216" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12483,11 +12481,11 @@
         <v>996</v>
       </c>
       <c r="J217" t="str">
-        <f>IF(G217=0,E217,IF(G217=1,F217,""))</f>
+        <f t="shared" si="6"/>
         <v>The artist's work isn't recognizable</v>
       </c>
       <c r="K217" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12520,11 +12518,11 @@
         <v>1005</v>
       </c>
       <c r="J218" t="str">
-        <f>IF(G218=0,E218,IF(G218=1,F218,""))</f>
+        <f t="shared" si="6"/>
         <v>He works really hard</v>
       </c>
       <c r="K218" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12557,11 +12555,11 @@
         <v>1006</v>
       </c>
       <c r="J219" t="str">
-        <f>IF(G219=0,E219,IF(G219=1,F219,""))</f>
+        <f t="shared" si="6"/>
         <v>He doesn't work really hard</v>
       </c>
       <c r="K219" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12594,11 +12592,11 @@
         <v>1015</v>
       </c>
       <c r="J220" t="str">
-        <f>IF(G220=0,E220,IF(G220=1,F220,""))</f>
+        <f t="shared" si="6"/>
         <v>He can jump really well</v>
       </c>
       <c r="K220" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12631,11 +12629,11 @@
         <v>1016</v>
       </c>
       <c r="J221" t="str">
-        <f>IF(G221=0,E221,IF(G221=1,F221,""))</f>
+        <f t="shared" si="6"/>
         <v>He can't jump really well</v>
       </c>
       <c r="K221" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12668,11 +12666,11 @@
         <v>1025</v>
       </c>
       <c r="J222" t="str">
-        <f>IF(G222=0,E222,IF(G222=1,F222,""))</f>
+        <f t="shared" si="6"/>
         <v>The love was very passionate</v>
       </c>
       <c r="K222" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12705,11 +12703,11 @@
         <v>1026</v>
       </c>
       <c r="J223" t="str">
-        <f>IF(G223=0,E223,IF(G223=1,F223,""))</f>
+        <f t="shared" si="6"/>
         <v>The love was not very passionate</v>
       </c>
       <c r="K223" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12742,11 +12740,11 @@
         <v>1035</v>
       </c>
       <c r="J224" t="str">
-        <f>IF(G224=0,E224,IF(G224=1,F224,""))</f>
+        <f t="shared" si="6"/>
         <v>The invention was very well done</v>
       </c>
       <c r="K224" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12779,11 +12777,11 @@
         <v>1036</v>
       </c>
       <c r="J225" t="str">
-        <f>IF(G225=0,E225,IF(G225=1,F225,""))</f>
+        <f t="shared" si="6"/>
         <v>The invention was not very well done</v>
       </c>
       <c r="K225" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12816,11 +12814,11 @@
         <v>1044</v>
       </c>
       <c r="J226" t="str">
-        <f>IF(G226=0,E226,IF(G226=1,F226,""))</f>
+        <f t="shared" si="6"/>
         <v>The boy is not a genius</v>
       </c>
       <c r="K226" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12853,11 +12851,11 @@
         <v>1045</v>
       </c>
       <c r="J227" t="str">
-        <f>IF(G227=0,E227,IF(G227=1,F227,""))</f>
+        <f t="shared" si="6"/>
         <v>The boy is a genius</v>
       </c>
       <c r="K227" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12890,11 +12888,11 @@
         <v>1053</v>
       </c>
       <c r="J228" t="str">
-        <f>IF(G228=0,E228,IF(G228=1,F228,""))</f>
+        <f t="shared" si="6"/>
         <v>they are hyped</v>
       </c>
       <c r="K228" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -12927,11 +12925,11 @@
         <v>1054</v>
       </c>
       <c r="J229" t="str">
-        <f>IF(G229=0,E229,IF(G229=1,F229,""))</f>
+        <f t="shared" si="6"/>
         <v>they aren't hyped</v>
       </c>
       <c r="K229" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -12964,11 +12962,11 @@
         <v>1062</v>
       </c>
       <c r="J230" t="str">
-        <f>IF(G230=0,E230,IF(G230=1,F230,""))</f>
+        <f t="shared" si="6"/>
         <v>The blanket does not keep me warm</v>
       </c>
       <c r="K230" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13001,11 +12999,11 @@
         <v>1063</v>
       </c>
       <c r="J231" t="str">
-        <f>IF(G231=0,E231,IF(G231=1,F231,""))</f>
+        <f t="shared" si="6"/>
         <v>The blanket keeps me warm</v>
       </c>
       <c r="K231" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13038,11 +13036,11 @@
         <v>1072</v>
       </c>
       <c r="J232" t="str">
-        <f>IF(G232=0,E232,IF(G232=1,F232,""))</f>
+        <f t="shared" si="6"/>
         <v>The music is not calming</v>
       </c>
       <c r="K232" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13075,11 +13073,11 @@
         <v>1073</v>
       </c>
       <c r="J233" t="str">
-        <f>IF(G233=0,E233,IF(G233=1,F233,""))</f>
+        <f t="shared" si="6"/>
         <v>The music is calming</v>
       </c>
       <c r="K233" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13112,11 +13110,11 @@
         <v>1081</v>
       </c>
       <c r="J234" t="str">
-        <f>IF(G234=0,E234,IF(G234=1,F234,""))</f>
+        <f t="shared" si="6"/>
         <v>The route followed a straight line</v>
       </c>
       <c r="K234" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13149,11 +13147,11 @@
         <v>1082</v>
       </c>
       <c r="J235" t="str">
-        <f>IF(G235=0,E235,IF(G235=1,F235,""))</f>
+        <f t="shared" si="6"/>
         <v>The route did not follow a straight line</v>
       </c>
       <c r="K235" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13186,11 +13184,11 @@
         <v>1091</v>
       </c>
       <c r="J236" t="str">
-        <f>IF(G236=0,E236,IF(G236=1,F236,""))</f>
+        <f t="shared" si="6"/>
         <v>The knife was sharp</v>
       </c>
       <c r="K236" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13223,11 +13221,11 @@
         <v>1092</v>
       </c>
       <c r="J237" t="str">
-        <f>IF(G237=0,E237,IF(G237=1,F237,""))</f>
+        <f t="shared" si="6"/>
         <v>The knife wasn't sharp</v>
       </c>
       <c r="K237" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13260,11 +13258,11 @@
         <v>1101</v>
       </c>
       <c r="J238" t="str">
-        <f>IF(G238=0,E238,IF(G238=1,F238,""))</f>
+        <f t="shared" si="6"/>
         <v>He's very serious</v>
       </c>
       <c r="K238" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13297,11 +13295,11 @@
         <v>1102</v>
       </c>
       <c r="J239" t="str">
-        <f>IF(G239=0,E239,IF(G239=1,F239,""))</f>
+        <f t="shared" si="6"/>
         <v>He's not very serious</v>
       </c>
       <c r="K239" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13334,11 +13332,11 @@
         <v>1111</v>
       </c>
       <c r="J240" t="str">
-        <f>IF(G240=0,E240,IF(G240=1,F240,""))</f>
+        <f t="shared" si="6"/>
         <v>The document is official</v>
       </c>
       <c r="K240" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13371,11 +13369,11 @@
         <v>1112</v>
       </c>
       <c r="J241" t="str">
-        <f>IF(G241=0,E241,IF(G241=1,F241,""))</f>
+        <f t="shared" si="6"/>
         <v>The document isn't official</v>
       </c>
       <c r="K241" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13408,11 +13406,11 @@
         <v>1121</v>
       </c>
       <c r="J242" t="str">
-        <f>IF(G242=0,E242,IF(G242=1,F242,""))</f>
+        <f t="shared" si="6"/>
         <v>The milk was not cold</v>
       </c>
       <c r="K242" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13445,11 +13443,11 @@
         <v>1122</v>
       </c>
       <c r="J243" t="str">
-        <f>IF(G243=0,E243,IF(G243=1,F243,""))</f>
+        <f t="shared" si="6"/>
         <v>The milk was cold</v>
       </c>
       <c r="K243" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13482,11 +13480,11 @@
         <v>1131</v>
       </c>
       <c r="J244" t="str">
-        <f>IF(G244=0,E244,IF(G244=1,F244,""))</f>
+        <f t="shared" si="6"/>
         <v>He is not a clean person</v>
       </c>
       <c r="K244" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13519,11 +13517,11 @@
         <v>1132</v>
       </c>
       <c r="J245" t="str">
-        <f>IF(G245=0,E245,IF(G245=1,F245,""))</f>
+        <f t="shared" si="6"/>
         <v>He is a clean person</v>
       </c>
       <c r="K245" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13556,11 +13554,11 @@
         <v>1141</v>
       </c>
       <c r="J246" t="str">
-        <f>IF(G246=0,E246,IF(G246=1,F246,""))</f>
+        <f t="shared" si="6"/>
         <v>The night was dark</v>
       </c>
       <c r="K246" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13593,11 +13591,11 @@
         <v>1142</v>
       </c>
       <c r="J247" t="str">
-        <f>IF(G247=0,E247,IF(G247=1,F247,""))</f>
+        <f t="shared" si="6"/>
         <v>The night was not dark</v>
       </c>
       <c r="K247" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13630,11 +13628,11 @@
         <v>1150</v>
       </c>
       <c r="J248" t="str">
-        <f>IF(G248=0,E248,IF(G248=1,F248,""))</f>
+        <f t="shared" si="6"/>
         <v>The food can be digested easily</v>
       </c>
       <c r="K248" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13667,11 +13665,11 @@
         <v>1151</v>
       </c>
       <c r="J249" t="str">
-        <f>IF(G249=0,E249,IF(G249=1,F249,""))</f>
+        <f t="shared" si="6"/>
         <v>The food can not be digested easily</v>
       </c>
       <c r="K249" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13704,11 +13702,11 @@
         <v>1158</v>
       </c>
       <c r="J250" t="str">
-        <f>IF(G250=0,E250,IF(G250=1,F250,""))</f>
+        <f t="shared" si="6"/>
         <v>Mary is a good singer</v>
       </c>
       <c r="K250" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13741,11 +13739,11 @@
         <v>1159</v>
       </c>
       <c r="J251" t="str">
-        <f>IF(G251=0,E251,IF(G251=1,F251,""))</f>
+        <f t="shared" si="6"/>
         <v>Mary is not a good singer</v>
       </c>
       <c r="K251" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13778,11 +13776,11 @@
         <v>1167</v>
       </c>
       <c r="J252" t="str">
-        <f>IF(G252=0,E252,IF(G252=1,F252,""))</f>
+        <f t="shared" si="6"/>
         <v>The illness is not serious</v>
       </c>
       <c r="K252" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13815,11 +13813,11 @@
         <v>1168</v>
       </c>
       <c r="J253" t="str">
-        <f>IF(G253=0,E253,IF(G253=1,F253,""))</f>
+        <f t="shared" si="6"/>
         <v>The illness is serious</v>
       </c>
       <c r="K253" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13852,11 +13850,11 @@
         <v>1179</v>
       </c>
       <c r="J254" t="str">
-        <f>IF(G254=0,E254,IF(G254=1,F254,""))</f>
+        <f t="shared" si="6"/>
         <v>The story was not enthralling</v>
       </c>
       <c r="K254" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>
@@ -13889,11 +13887,11 @@
         <v>1180</v>
       </c>
       <c r="J255" t="str">
-        <f>IF(G255=0,E255,IF(G255=1,F255,""))</f>
+        <f t="shared" si="6"/>
         <v>The story was enthralling</v>
       </c>
       <c r="K255" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13926,11 +13924,11 @@
         <v>1187</v>
       </c>
       <c r="J256" t="str">
-        <f>IF(G256=0,E256,IF(G256=1,F256,""))</f>
+        <f t="shared" si="6"/>
         <v>That monster was scary</v>
       </c>
       <c r="K256" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>intens</v>
       </c>
     </row>
@@ -13963,11 +13961,11 @@
         <v>1188</v>
       </c>
       <c r="J257" t="str">
-        <f>IF(G257=0,E257,IF(G257=1,F257,""))</f>
+        <f t="shared" si="6"/>
         <v>That monster was not scary</v>
       </c>
       <c r="K257" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>neg</v>
       </c>
     </row>

</xml_diff>